<commit_message>
feat: Implement bulk campaign feature with CSV upload and Outbox UI
</commit_message>
<xml_diff>
--- a/WhatsApp_Numbers.xlsx
+++ b/WhatsApp_Numbers.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Atoms Group\Atoms Digital Solutions\Software\WhatsApp Integration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\NextJs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA24C237-477A-4B26-BB54-88160FB09BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5B549F8F-CE4C-4FE6-8D23-4083E35A2D75}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2350" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,16 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Country Code</t>
-  </si>
-  <si>
-    <t>Contact Number</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Sravanth</t>
   </si>
@@ -57,19 +47,22 @@
     <t>Sravan</t>
   </si>
   <si>
-    <t>Atoms Office</t>
-  </si>
-  <si>
     <t>Prudhvi</t>
   </si>
   <si>
     <t>Azaruddin</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>whatsappnumber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -414,139 +407,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62F462B-A252-43FC-AE51-47E550C07A52}">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>918688275808</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>917331153737</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>919703394393</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>91</v>
-      </c>
-      <c r="B2">
-        <v>8688275808</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>918885839339</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>91</v>
-      </c>
-      <c r="B3">
-        <v>7331153737</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>917331163737</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>91</v>
-      </c>
-      <c r="B4">
-        <v>9703394393</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>919951709347</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>91</v>
-      </c>
-      <c r="B5">
-        <v>8885839339</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>917330802181</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>91</v>
-      </c>
-      <c r="B6">
-        <v>7331163737</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>919381048977</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>91</v>
-      </c>
-      <c r="B7">
-        <v>9951709347</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>919052131350</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>91</v>
-      </c>
-      <c r="B8">
-        <v>7330802181</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>91</v>
-      </c>
-      <c r="B9">
-        <v>7396743341</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>91</v>
-      </c>
-      <c r="B10">
-        <v>9381048977</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>91</v>
-      </c>
-      <c r="B11">
-        <v>9052131350</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>